<commit_message>
Updated color scheme and labels
</commit_message>
<xml_diff>
--- a/projects/va_emerging_tech/jbennett_dissertation/data/data_va_noEmissionLimit.xlsx
+++ b/projects/va_emerging_tech/jbennett_dissertation/data/data_va_noEmissionLimit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89310018-9148-4E44-9303-86863365793D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2D13FF-8A4F-405A-B922-B495AE768B74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="844" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -5238,8 +5238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -6639,9 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>

</xml_diff>